<commit_message>
Sync with student every 5 secs
</commit_message>
<xml_diff>
--- a/SRC/src/yatuedx/documentation/project plan/Tasks.xlsx
+++ b/SRC/src/yatuedx/documentation/project plan/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\yatuedu\YatuEdu\SRC\src\yatuedx\documentation\project plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6195336-3D33-4DA8-802B-1D8AC08949D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F71B157-2A25-4324-A556-9163E650EB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CF81CB7-F560-4DDC-BC41-500716B0F4AB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>Issue</t>
   </si>
@@ -61,15 +61,9 @@
     <t>Lian</t>
   </si>
   <si>
-    <t>New Function</t>
-  </si>
-  <si>
     <t>Sync board</t>
   </si>
   <si>
-    <t>Use a timer to sync every 3 seconds</t>
-  </si>
-  <si>
     <t>Created by Day</t>
   </si>
   <si>
@@ -91,12 +85,6 @@
     <t>Old code has to explicitly add audio tag. If you do not want video?</t>
   </si>
   <si>
-    <t>Auto Sync</t>
-  </si>
-  <si>
-    <t>Automatically check content of student and teacher and sync if difference found</t>
-  </si>
-  <si>
     <t>finMind</t>
   </si>
   <si>
@@ -215,13 +203,64 @@
   </si>
   <si>
     <t>We need to have Java code run at the server in a sandbox securely.  Please come up with a plan on how to do it.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Sync with each student</t>
+  </si>
+  <si>
+    <t>Lain</t>
+  </si>
+  <si>
+    <t>Use a timer to sync every 5 seconds</t>
+  </si>
+  <si>
+    <t>USE a timer to sync every 10  seconds to check hash of the content an to make sure we are in sync</t>
+  </si>
+  <si>
+    <t>Task 2</t>
+  </si>
+  <si>
+    <t>Task 1</t>
+  </si>
+  <si>
+    <t>Need to sync with students who has partial content. Task  2</t>
+  </si>
+  <si>
+    <t>Task 3</t>
+  </si>
+  <si>
+    <t>During exercise, obtain student board content on deman</t>
+  </si>
+  <si>
+    <t>Task 4</t>
+  </si>
+  <si>
+    <t>Task 5</t>
+  </si>
+  <si>
+    <t>Task 6</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t>Task 8</t>
+  </si>
+  <si>
+    <t>Task 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +315,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -297,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -316,6 +362,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +680,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +690,9 @@
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="38.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="77.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -664,15 +713,22 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2"/>
       <c r="E2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -696,10 +752,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4">
         <v>44583</v>
@@ -710,19 +766,19 @@
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4">
         <v>44577</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" s="5">
         <v>44576</v>
@@ -738,10 +794,10 @@
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -750,7 +806,7 @@
         <v>44582</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F8" s="5">
         <v>44581</v>
@@ -766,12 +822,12 @@
       <c r="D10" s="4"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -780,44 +836,52 @@
         <v>44583</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F11" s="5">
         <v>44576</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5">
-        <v>44590</v>
-      </c>
-      <c r="F12" s="5">
-        <v>44576</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D12" s="4">
+        <v>44584</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="5">
-        <v>44597</v>
+        <v>44590</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="F13" s="5">
         <v>44576</v>
@@ -825,86 +889,89 @@
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F14" s="5">
         <v>44590</v>
       </c>
       <c r="I14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F19" s="5">
         <v>44597</v>
@@ -918,25 +985,25 @@
     </row>
     <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -962,77 +1029,77 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added student dashboard on teacher s panel
</commit_message>
<xml_diff>
--- a/SRC/src/yatuedx/documentation/project plan/Tasks.xlsx
+++ b/SRC/src/yatuedx/documentation/project plan/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\yatuedu\YatuEdu\SRC\src\yatuedx\documentation\project plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F71B157-2A25-4324-A556-9163E650EB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861701D9-B2F4-40D9-85CE-DC984DA81D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CF81CB7-F560-4DDC-BC41-500716B0F4AB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>Issue</t>
   </si>
@@ -85,12 +85,6 @@
     <t>Old code has to explicitly add audio tag. If you do not want video?</t>
   </si>
   <si>
-    <t>finMind</t>
-  </si>
-  <si>
-    <t>TASK</t>
-  </si>
-  <si>
     <t>ADD ERROR PAGE (MESSAGES)</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>Save home work</t>
   </si>
   <si>
-    <t>Fix wizard term-perm option</t>
-  </si>
-  <si>
     <t>From application to pipeline</t>
   </si>
   <si>
@@ -214,9 +205,6 @@
     <t>Sync with each student</t>
   </si>
   <si>
-    <t>Lain</t>
-  </si>
-  <si>
     <t>Use a timer to sync every 5 seconds</t>
   </si>
   <si>
@@ -254,6 +242,30 @@
   </si>
   <si>
     <t>Task 9</t>
+  </si>
+  <si>
+    <t>Issue 1</t>
+  </si>
+  <si>
+    <t>User Name should be w/o special chars since we use it as video id</t>
+  </si>
+  <si>
+    <t>Issue 2</t>
+  </si>
+  <si>
+    <t>Timer not working every time</t>
+  </si>
+  <si>
+    <t>lian</t>
+  </si>
+  <si>
+    <t>Task  10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add student name tag on top of student cosole </t>
+  </si>
+  <si>
+    <t>Add a name tag to identify student. Especially useful when multiple students are present</t>
   </si>
 </sst>
 </file>
@@ -677,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F16FB91-AA76-4F98-95A8-6495A23F792D}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,15 +728,15 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2"/>
       <c r="E2" s="2"/>
@@ -746,6 +758,9 @@
       <c r="F3" s="5">
         <v>44576</v>
       </c>
+      <c r="G3" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -794,10 +809,10 @@
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -806,7 +821,7 @@
         <v>44582</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F8" s="5">
         <v>44581</v>
@@ -824,7 +839,7 @@
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -836,7 +851,7 @@
         <v>44583</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F11" s="5">
         <v>44576</v>
@@ -845,31 +860,31 @@
         <v>0.99</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D12" s="4">
         <v>44584</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>10</v>
@@ -881,129 +896,161 @@
         <v>44590</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F13" s="5">
         <v>44576</v>
       </c>
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F14" s="5">
         <v>44590</v>
       </c>
       <c r="I14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F19" s="5">
         <v>44597</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="4">
+        <v>44586</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>26</v>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1029,77 +1076,77 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated login and register html
</commit_message>
<xml_diff>
--- a/SRC/src/yatuedx/documentation/project plan/Tasks.xlsx
+++ b/SRC/src/yatuedx/documentation/project plan/Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\yatuedu\YatuEdu\SRC\src\yatuedx\documentation\project plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5378443-84B2-4B73-B90C-3D2E80FA30DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BB0E06-7CEE-4890-9342-3CFC879D5B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CF81CB7-F560-4DDC-BC41-500716B0F4AB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Issue</t>
   </si>
@@ -275,6 +275,15 @@
   </si>
   <si>
     <t>80% (need to test)</t>
+  </si>
+  <si>
+    <t>Task 11</t>
+  </si>
+  <si>
+    <t>Sync to teacher's mode when joining the class</t>
+  </si>
+  <si>
+    <t>Now we set the exercise mode, but this not desirable since we don't know which mode to switch to if a student is late</t>
   </si>
 </sst>
 </file>
@@ -704,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F16FB91-AA76-4F98-95A8-6495A23F792D}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,33 +1065,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="13">
+      <c r="E21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="4">
+        <v>44598</v>
+      </c>
+      <c r="G21" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
+      <c r="G22" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
@@ -1090,13 +1116,16 @@
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+    <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjusted student UI with tabs and saved spaces
</commit_message>
<xml_diff>
--- a/SRC/src/yatuedx/documentation/project plan/Tasks.xlsx
+++ b/SRC/src/yatuedx/documentation/project plan/Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\yatuedu\YatuEdu\SRC\src\yatuedx\documentation\project plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9465724A-3D20-41E1-8686-91E2E54248C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56CDAAF-D287-4E85-81DD-900DD43443AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CF81CB7-F560-4DDC-BC41-500716B0F4AB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="100">
   <si>
     <t>Issue</t>
   </si>
@@ -290,13 +290,58 @@
   </si>
   <si>
     <t>Sync Board should forcefully sync content to all student regardless mode</t>
+  </si>
+  <si>
+    <t>Copy student code to board</t>
+  </si>
+  <si>
+    <t>Task 12</t>
+  </si>
+  <si>
+    <t>Task 13</t>
+  </si>
+  <si>
+    <t>Enlarge shared screen</t>
+  </si>
+  <si>
+    <t>Task 14</t>
+  </si>
+  <si>
+    <t>Re-arrange tool buttons for students</t>
+  </si>
+  <si>
+    <t>Task 15</t>
+  </si>
+  <si>
+    <t>Using tabs to present multiple consoles below backboard</t>
+  </si>
+  <si>
+    <t>Task 16</t>
+  </si>
+  <si>
+    <t>Doing task 15 for teachers</t>
+  </si>
+  <si>
+    <t>100% (obsolete)</t>
+  </si>
+  <si>
+    <t>Task 17</t>
+  </si>
+  <si>
+    <t>Obtain Share Screen Event and inform Students to enlarge their screen</t>
+  </si>
+  <si>
+    <t>Student receives messages from teacher and display</t>
+  </si>
+  <si>
+    <t>Task 18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +403,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -379,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -405,6 +465,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F16FB91-AA76-4F98-95A8-6495A23F792D}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,8 +1032,8 @@
       <c r="F14" s="5">
         <v>44590</v>
       </c>
-      <c r="G14" s="13">
-        <v>0.5</v>
+      <c r="G14" s="12">
+        <v>1</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
@@ -988,8 +1052,8 @@
       <c r="E15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="13">
-        <v>0</v>
+      <c r="G15" s="12">
+        <v>1</v>
       </c>
       <c r="I15" t="s">
         <v>25</v>
@@ -1002,8 +1066,8 @@
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="13">
-        <v>0</v>
+      <c r="G16" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1101,8 +1165,8 @@
       <c r="C22" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="13">
-        <v>0</v>
+      <c r="G22" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1126,8 +1190,8 @@
       <c r="C24" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="13">
-        <v>0</v>
+      <c r="G24" s="12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -1147,6 +1211,77 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" s="13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>